<commit_message>
nomenclatura custo x custeio
</commit_message>
<xml_diff>
--- a/uorgs_descentralizadas.xlsx
+++ b/uorgs_descentralizadas.xlsx
@@ -400,8 +400,10 @@
           <t>SERVIC APOIO ADMINST DESCENTRALIZADA-AL</t>
         </is>
       </c>
-      <c r="D2">
-        <v>304912</v>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>304912</t>
+        </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -425,8 +427,10 @@
           <t>SUPERINTENDENCIA DE ADMINISTRACAO MF/AL</t>
         </is>
       </c>
-      <c r="D3">
-        <v>202690</v>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>202690</t>
+        </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -450,8 +454,10 @@
           <t>DIVISAO DE GESTAO DE PESSOAS</t>
         </is>
       </c>
-      <c r="D4">
-        <v>280633</v>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>280633</t>
+        </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -475,8 +481,10 @@
           <t>DIVISAO DE GESTAO DE PESSOAS/SAMF/AM</t>
         </is>
       </c>
-      <c r="D5">
-        <v>212667</v>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>212667</t>
+        </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -500,8 +508,10 @@
           <t>DIVISAO DE ORCAMENTOS E FINANCAS</t>
         </is>
       </c>
-      <c r="D6">
-        <v>280634</v>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>280634</t>
+        </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -525,8 +535,10 @@
           <t>DIVISAO DE RECURSOS LOGISTICOS</t>
         </is>
       </c>
-      <c r="D7">
-        <v>280632</v>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>280632</t>
+        </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -550,8 +562,10 @@
           <t>DIVISAO DE RECURSOS LOGISTICOS/SAMF/AM</t>
         </is>
       </c>
-      <c r="D8">
-        <v>212665</v>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>212665</t>
+        </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -575,8 +589,10 @@
           <t>GEREN REG DE ADMIN EM AMAZONAS</t>
         </is>
       </c>
-      <c r="D9">
-        <v>278713</v>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>278713</t>
+        </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -600,8 +616,10 @@
           <t>SERVICO DE ATIVOS</t>
         </is>
       </c>
-      <c r="D10">
-        <v>280672</v>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>280672</t>
+        </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -625,8 +643,10 @@
           <t>SERVICO DE SUPRIMENTOS/DRL/SAMF/AM</t>
         </is>
       </c>
-      <c r="D11">
-        <v>212666</v>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>212666</t>
+        </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -650,8 +670,10 @@
           <t>SUPERINTENDENCIA DE ADMINISTRACAO MF/AM</t>
         </is>
       </c>
-      <c r="D12">
-        <v>202709</v>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>202709</t>
+        </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -675,8 +697,10 @@
           <t>SUPERINTENDENCIA DE ADMINISTRACAO MF/AP</t>
         </is>
       </c>
-      <c r="D13">
-        <v>202712</v>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>202712</t>
+        </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -700,8 +724,10 @@
           <t>DIVISAO DE GESTAO DE PESSOAS/BA</t>
         </is>
       </c>
-      <c r="D14">
-        <v>280636</v>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>280636</t>
+        </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -725,8 +751,10 @@
           <t>DIVISAO DE PLANEJAMENTO E ORCAMENTO/BA</t>
         </is>
       </c>
-      <c r="D15">
-        <v>280635</v>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>280635</t>
+        </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -750,8 +778,10 @@
           <t>DIVISAO DE RECURSOS LOGISTICOS/BA</t>
         </is>
       </c>
-      <c r="D16">
-        <v>280637</v>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>280637</t>
+        </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -775,8 +805,10 @@
           <t>SERVICO DE ATIVOS/BA</t>
         </is>
       </c>
-      <c r="D17">
-        <v>280695</v>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>280695</t>
+        </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -800,8 +832,10 @@
           <t>SERVICO DE ORCAMENTO E FINANCAS/BA</t>
         </is>
       </c>
-      <c r="D18">
-        <v>280667</v>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>280667</t>
+        </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -825,8 +859,10 @@
           <t>SUPERINT REG DE ADMIN NA BAHIA</t>
         </is>
       </c>
-      <c r="D19">
-        <v>278706</v>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>278706</t>
+        </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -850,8 +886,10 @@
           <t>SUPERINTENDENCIA DE ADMINISTRACAO MF/BA</t>
         </is>
       </c>
-      <c r="D20">
-        <v>202707</v>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>202707</t>
+        </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -875,8 +913,10 @@
           <t>DIV. DE PLANEJ. E CONTABILIDADE/SAMF/CE</t>
         </is>
       </c>
-      <c r="D21">
-        <v>212614</v>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>212614</t>
+        </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -900,8 +940,10 @@
           <t>DIVISAO DE GESTAO DE PESSOAS/CE</t>
         </is>
       </c>
-      <c r="D22">
-        <v>280638</v>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>280638</t>
+        </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -925,8 +967,10 @@
           <t>DIVISAO DE GESTAO DE PESSOAS/SAMF/CE</t>
         </is>
       </c>
-      <c r="D23">
-        <v>212618</v>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>212618</t>
+        </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -950,8 +994,10 @@
           <t>DIVISAO DE PLANEJAMENTO E ORCAMENTO/CE</t>
         </is>
       </c>
-      <c r="D24">
-        <v>280640</v>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>280640</t>
+        </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -975,8 +1021,10 @@
           <t>DIVISAO DE REC. LOGISTICOS/SAMF/CE</t>
         </is>
       </c>
-      <c r="D25">
-        <v>212616</v>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>212616</t>
+        </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -1000,8 +1048,10 @@
           <t>DIVISAO DE RECURSOS LOGISTICOS/CE</t>
         </is>
       </c>
-      <c r="D26">
-        <v>280639</v>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>280639</t>
+        </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -1025,8 +1075,10 @@
           <t>GERENCIA REGIONAL DE ADMINISTRACAO/CE</t>
         </is>
       </c>
-      <c r="D27">
-        <v>87101</v>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>87101</t>
+        </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -1050,8 +1102,10 @@
           <t>SERV. DE ORC. E FINANCAS/SAMF/CE</t>
         </is>
       </c>
-      <c r="D28">
-        <v>212615</v>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>212615</t>
+        </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1075,8 +1129,10 @@
           <t>SERVICO DE ATIVOS/CE</t>
         </is>
       </c>
-      <c r="D29">
-        <v>280669</v>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>280669</t>
+        </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1100,8 +1156,10 @@
           <t>SERVICO DE ATIVOS/DIGEP/SAMF/CE</t>
         </is>
       </c>
-      <c r="D30">
-        <v>212619</v>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>212619</t>
+        </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1125,8 +1183,10 @@
           <t>SERVICO DE INAT. E PENSION/DIGEP/SAMF/CE</t>
         </is>
       </c>
-      <c r="D31">
-        <v>212620</v>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>212620</t>
+        </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -1150,8 +1210,10 @@
           <t>SERVICO DE SUPRIMENTOS/CE</t>
         </is>
       </c>
-      <c r="D32">
-        <v>280668</v>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>280668</t>
+        </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -1175,8 +1237,10 @@
           <t>SERVICO DE SUPRIMENTOS/DRL/SAMF/CE</t>
         </is>
       </c>
-      <c r="D33">
-        <v>212617</v>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>212617</t>
+        </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1200,8 +1264,10 @@
           <t>SUPERINT REG DE ADMIN NO CEARA</t>
         </is>
       </c>
-      <c r="D34">
-        <v>278707</v>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>278707</t>
+        </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -1225,8 +1291,10 @@
           <t>SUPERINTENDENCIA DE ADMINISTRACAO MF/CE</t>
         </is>
       </c>
-      <c r="D35">
-        <v>202706</v>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>202706</t>
+        </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1250,8 +1318,10 @@
           <t>SUPERINTENDENCIA DE ADMINISTRACAO MF/DF</t>
         </is>
       </c>
-      <c r="D36">
-        <v>202689</v>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>202689</t>
+        </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1275,8 +1345,10 @@
           <t>GEREN REG DE ADMIN NO ESPIRITO SANTO</t>
         </is>
       </c>
-      <c r="D37">
-        <v>278716</v>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>278716</t>
+        </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -1297,15 +1369,17 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>REPRESENTACAO DA DPU/ES</t>
-        </is>
-      </c>
-      <c r="D38">
-        <v>74073</v>
+          <t>SERVIC APOIO ADMINST DESCENTRALIZADA-ES</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>304908</t>
+        </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>17000-000052239</t>
+          <t>17000-000071900</t>
         </is>
       </c>
     </row>
@@ -1322,40 +1396,44 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>SERVIC APOIO ADMINST DESCENTRALIZADA-ES</t>
-        </is>
-      </c>
-      <c r="D39">
-        <v>304908</v>
+          <t>SUPERINTENDENCIA DE ADMINISTRACAO MF/ES</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>202691</t>
+        </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>17000-000071900</t>
+          <t>17000-000061983</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>ES</t>
+          <t>GO</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>SAMF/ES</t>
+          <t>SAMF/GO</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>SUPERINTENDENCIA DE ADMINISTRACAO MF/ES</t>
-        </is>
-      </c>
-      <c r="D40">
-        <v>202691</v>
+          <t>GEREN REG DE ADM EM GOIAS E TOCANTINS</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>278717</t>
+        </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>17000-000061983</t>
+          <t>17000-000067389</t>
         </is>
       </c>
     </row>
@@ -1372,15 +1450,17 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>GEREN REG DE ADM EM GOIAS E TOCANTINS</t>
-        </is>
-      </c>
-      <c r="D41">
-        <v>278717</v>
+          <t>SERVIC APOIO ADMINST DESCENTRALIZADA-GO</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>304910</t>
+        </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>17000-000067389</t>
+          <t>17000-000071902</t>
         </is>
       </c>
     </row>
@@ -1397,40 +1477,44 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>SERVIC APOIO ADMINST DESCENTRALIZADA-GO</t>
-        </is>
-      </c>
-      <c r="D42">
-        <v>304910</v>
+          <t>SUPERINTENDENCIA DE ADMINISTRACAO MF/GO</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>202695</t>
+        </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>17000-000071902</t>
+          <t>17000-000061987</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>GO</t>
+          <t>MA</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>SAMF/GO</t>
+          <t>SAMF/MA</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>SUPERINTENDENCIA DE ADMINISTRACAO MF/GO</t>
-        </is>
-      </c>
-      <c r="D43">
-        <v>202695</v>
+          <t>GEREN REG DE ADMIN NO MARANHAO</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>278718</t>
+        </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>17000-000061987</t>
+          <t>17000-000067390</t>
         </is>
       </c>
     </row>
@@ -1447,15 +1531,17 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>GEREN REG DE ADMIN NO MARANHAO</t>
-        </is>
-      </c>
-      <c r="D44">
-        <v>278718</v>
+          <t>SERVIC APOIO ADMINST DESCENTRALIZADA-MA</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>304906</t>
+        </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>17000-000067390</t>
+          <t>17000-000071898</t>
         </is>
       </c>
     </row>
@@ -1472,40 +1558,44 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>SERVIC APOIO ADMINST DESCENTRALIZADA-MA</t>
-        </is>
-      </c>
-      <c r="D45">
-        <v>304906</v>
+          <t>SUPERINTENDENCIA DE ADMINISTRACAO MF/MA</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>202696</t>
+        </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>17000-000071898</t>
+          <t>17000-000061988</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>MA</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>SAMF/MA</t>
+          <t>SAMF/MG</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>SUPERINTENDENCIA DE ADMINISTRACAO MF/MA</t>
-        </is>
-      </c>
-      <c r="D46">
-        <v>202696</v>
+          <t>CASA DOS CONTOS/OURO PRETO/MG/SAMF</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>24313</t>
+        </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>17000-000061988</t>
+          <t>17000-000004517</t>
         </is>
       </c>
     </row>
@@ -1522,15 +1612,17 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>CASA DOS CONTOS/OURO PRETO/MG/SAMF</t>
-        </is>
-      </c>
-      <c r="D47">
-        <v>24313</v>
+          <t>DIV. DE PLANEJ. E CONTABILIDADE/SAMF/MG</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>212621</t>
+        </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>17000-000004517</t>
+          <t>17000-000063124</t>
         </is>
       </c>
     </row>
@@ -1547,15 +1639,17 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>DIV. DE PLANEJ. E CONTABILIDADE/SAMF/MG</t>
-        </is>
-      </c>
-      <c r="D48">
-        <v>212621</v>
+          <t>DIVISAO DE GESTAO DE PESSOAS/MG</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>280644</t>
+        </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>17000-000063124</t>
+          <t>17000-000069316</t>
         </is>
       </c>
     </row>
@@ -1572,15 +1666,17 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>DIVISAO DE GESTAO DE PESSOAS/MG</t>
-        </is>
-      </c>
-      <c r="D49">
-        <v>280644</v>
+          <t>DIVISAO DE GESTAO DE PESSOAS/SAMF/MG</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>212625</t>
+        </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>17000-000069316</t>
+          <t>17000-000063128</t>
         </is>
       </c>
     </row>
@@ -1597,15 +1693,17 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>DIVISAO DE GESTAO DE PESSOAS/SAMF/MG</t>
-        </is>
-      </c>
-      <c r="D50">
-        <v>212625</v>
+          <t>DIVISAO DE PLANEJAMENTO E ORCAMENTO/MG</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>280642</t>
+        </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>17000-000063128</t>
+          <t>17000-000069314</t>
         </is>
       </c>
     </row>
@@ -1622,15 +1720,17 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>DIVISAO DE PLANEJAMENTO E ORCAMENTO/MG</t>
-        </is>
-      </c>
-      <c r="D51">
-        <v>280642</v>
+          <t>DIVISAO DE REC. LOGISTICOS/SAMF/MG</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>212623</t>
+        </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>17000-000069314</t>
+          <t>17000-000063126</t>
         </is>
       </c>
     </row>
@@ -1647,15 +1747,17 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>DIVISAO DE REC. LOGISTICOS/SAMF/MG</t>
-        </is>
-      </c>
-      <c r="D52">
-        <v>212623</v>
+          <t>DIVISAO DE RECURSOS LOGISTICOS/MG</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>280643</t>
+        </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>17000-000063126</t>
+          <t>17000-000069315</t>
         </is>
       </c>
     </row>
@@ -1672,15 +1774,17 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>DIVISAO DE RECURSOS LOGISTICOS/MG</t>
-        </is>
-      </c>
-      <c r="D53">
-        <v>280643</v>
+          <t>SERVICO DE ORC. E FINANCAS/SAMF/MG</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>212622</t>
+        </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>17000-000069315</t>
+          <t>17000-000063125</t>
         </is>
       </c>
     </row>
@@ -1697,15 +1801,17 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>SERVICO DE ORC. E FINANCAS/SAMF/MG</t>
-        </is>
-      </c>
-      <c r="D54">
-        <v>212622</v>
+          <t>SERVICO DE ORCAMENTO E FINANCAS/MG</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>280670</t>
+        </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>17000-000063125</t>
+          <t>17000-000069342</t>
         </is>
       </c>
     </row>
@@ -1722,15 +1828,17 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>SERVICO DE ORCAMENTO E FINANCAS/MG</t>
-        </is>
-      </c>
-      <c r="D55">
-        <v>280670</v>
+          <t>SERVICO DE SUPRIMENTOS/DRL/SAMF/MG</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>212624</t>
+        </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>17000-000069342</t>
+          <t>17000-000063127</t>
         </is>
       </c>
     </row>
@@ -1747,15 +1855,17 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>SERVICO DE SUPRIMENTOS/DRL/SAMF/MG</t>
-        </is>
-      </c>
-      <c r="D56">
-        <v>212624</v>
+          <t>SERVICO DE SUPRIMENTOS/MG</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>280671</t>
+        </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>17000-000063127</t>
+          <t>17000-000069343</t>
         </is>
       </c>
     </row>
@@ -1772,15 +1882,17 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>SERVICO DE SUPRIMENTOS/MG</t>
-        </is>
-      </c>
-      <c r="D57">
-        <v>280671</v>
+          <t>SUPERINT REG DE ADMIN EM MINAS GERAIS</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>278701</t>
+        </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>17000-000069343</t>
+          <t>17000-000067373</t>
         </is>
       </c>
     </row>
@@ -1797,40 +1909,44 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>SUPERINT REG DE ADMIN EM MINAS GERAIS</t>
-        </is>
-      </c>
-      <c r="D58">
-        <v>278701</v>
+          <t>SUPERINTENDENCIA DE ADMINISTRACAO MF/MG</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>202693</t>
+        </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>17000-000067373</t>
+          <t>17000-000061985</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>MG</t>
+          <t>MS</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>SAMF/MG</t>
+          <t>SAMF/MS</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>SUPERINTENDENCIA DE ADMINISTRACAO MF/MG</t>
-        </is>
-      </c>
-      <c r="D59">
-        <v>202693</v>
+          <t>GEREN REG DE ADMIN NO MATO GROSSO DO SUL</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>278719</t>
+        </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>17000-000061985</t>
+          <t>17000-000067391</t>
         </is>
       </c>
     </row>
@@ -1847,15 +1963,17 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>GEREN REG DE ADMIN NO MATO GROSSO DO SUL</t>
-        </is>
-      </c>
-      <c r="D60">
-        <v>278719</v>
+          <t>SERV. APOIO ADM. DESCENTRALIZADA-MS</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>304904</t>
+        </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>17000-000067391</t>
+          <t>17000-000071896</t>
         </is>
       </c>
     </row>
@@ -1872,40 +1990,44 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>SERV. APOIO ADM. DESCENTRALIZADA-MS</t>
-        </is>
-      </c>
-      <c r="D61">
-        <v>304904</v>
+          <t>SUPERINTENDENCIA DE ADMINISTRACAO MF/MS</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>202697</t>
+        </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>17000-000071896</t>
+          <t>17000-000061989</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>MS</t>
+          <t>MT</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>SAMF/MS</t>
+          <t>SAMF/MT</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>SUPERINTENDENCIA DE ADMINISTRACAO MF/MS</t>
-        </is>
-      </c>
-      <c r="D62">
-        <v>202697</v>
+          <t>DIV DE PLANEJ, ORCAMENTO E FINANCAS/MT</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>280648</t>
+        </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>17000-000061989</t>
+          <t>17000-000069320</t>
         </is>
       </c>
     </row>
@@ -1922,15 +2044,17 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>DIV DE PLANEJ, ORCAMENTO E FINANCAS/MT</t>
-        </is>
-      </c>
-      <c r="D63">
-        <v>280648</v>
+          <t>DIV. DE REC. LOGISTICOS/SAMF/MT</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>212671</t>
+        </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>17000-000069320</t>
+          <t>17000-000063174</t>
         </is>
       </c>
     </row>
@@ -1947,15 +2071,17 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>DIV. DE REC. LOGISTICOS/SAMF/MT</t>
-        </is>
-      </c>
-      <c r="D64">
-        <v>212671</v>
+          <t>DIVIS¶O PLANEJ., ORŠAMENTO E FINANŠAS</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>212669</t>
+        </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>17000-000063174</t>
+          <t>17000-000063172</t>
         </is>
       </c>
     </row>
@@ -1972,15 +2098,17 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>DIVIS¶O PLANEJ., ORŠAMENTO E FINANŠAS</t>
-        </is>
-      </c>
-      <c r="D65">
-        <v>212669</v>
+          <t>DIVISAO DE GESTAO DE PESSOAS/MT</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>280647</t>
+        </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>17000-000063172</t>
+          <t>17000-000069319</t>
         </is>
       </c>
     </row>
@@ -1997,15 +2125,17 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>DIVISAO DE GESTAO DE PESSOAS/MT</t>
-        </is>
-      </c>
-      <c r="D66">
-        <v>280647</v>
+          <t>DIVISAO DE GESTAO DE PESSOAS/SAMF/MT</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>212673</t>
+        </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>17000-000069319</t>
+          <t>17000-000063176</t>
         </is>
       </c>
     </row>
@@ -2022,15 +2152,17 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>DIVISAO DE GESTAO DE PESSOAS/SAMF/MT</t>
-        </is>
-      </c>
-      <c r="D67">
-        <v>212673</v>
+          <t>DIVISAO DE RECURSOS LOGISTICOS/MT</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>280646</t>
+        </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>17000-000063176</t>
+          <t>17000-000069318</t>
         </is>
       </c>
     </row>
@@ -2047,15 +2179,17 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>DIVISAO DE RECURSOS LOGISTICOS/MT</t>
-        </is>
-      </c>
-      <c r="D68">
-        <v>280646</v>
+          <t>GEREN REG DE ADMIN NO MATO GROSSO</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>278714</t>
+        </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>17000-000069318</t>
+          <t>17000-000067386</t>
         </is>
       </c>
     </row>
@@ -2072,15 +2206,17 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>GEREN REG DE ADMIN NO MATO GROSSO</t>
-        </is>
-      </c>
-      <c r="D69">
-        <v>278714</v>
+          <t>SERVICO DE ATIVOS/DIGEP/SAMF/MT</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>212674</t>
+        </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>17000-000067386</t>
+          <t>17000-000063177</t>
         </is>
       </c>
     </row>
@@ -2097,15 +2233,17 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>SERVICO DE ATIVOS/DIGEP/SAMF/MT</t>
-        </is>
-      </c>
-      <c r="D70">
-        <v>212674</v>
+          <t>SERVICO DE ATIVOS/MT</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>280676</t>
+        </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>17000-000063177</t>
+          <t>17000-000069348</t>
         </is>
       </c>
     </row>
@@ -2122,15 +2260,17 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>SERVICO DE ATIVOS/MT</t>
-        </is>
-      </c>
-      <c r="D71">
-        <v>280676</v>
+          <t>SERVICO DE SUPRIMENTOS/DRL/SAMF/MT</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>212672</t>
+        </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>17000-000069348</t>
+          <t>17000-000063175</t>
         </is>
       </c>
     </row>
@@ -2147,40 +2287,44 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>SERVICO DE SUPRIMENTOS/DRL/SAMF/MT</t>
-        </is>
-      </c>
-      <c r="D72">
-        <v>212672</v>
+          <t>SUPERINTENDENCIA DE ADMINISTRACAO MF/MT</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>202710</t>
+        </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>17000-000063175</t>
+          <t>17000-000062002</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>MT</t>
+          <t>PA</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>SAMF/MT</t>
+          <t>SAMF/PA</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>SUPERINTENDENCIA DE ADMINISTRACAO MF/MT</t>
-        </is>
-      </c>
-      <c r="D73">
-        <v>202710</v>
+          <t>DIV DE PLANEJ, ORCAMENTO E FINANCAS/PA</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>280651</t>
+        </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>17000-000062002</t>
+          <t>17000-000069323</t>
         </is>
       </c>
     </row>
@@ -2197,15 +2341,17 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>DIV DE PLANEJ, ORCAMENTO E FINANCAS/PA</t>
-        </is>
-      </c>
-      <c r="D74">
-        <v>280651</v>
+          <t>DIV. DE REC. LOGISTICOS/SAMF/PA</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>212630</t>
+        </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>17000-000069323</t>
+          <t>17000-000063133</t>
         </is>
       </c>
     </row>
@@ -2222,15 +2368,17 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>DIV. DE REC. LOGISTICOS/SAMF/PA</t>
-        </is>
-      </c>
-      <c r="D75">
-        <v>212630</v>
+          <t>DIVISAO DE GESTAO DE PESSOAS/PA</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>280649</t>
+        </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>17000-000063133</t>
+          <t>17000-000069321</t>
         </is>
       </c>
     </row>
@@ -2247,15 +2395,17 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>DIVISAO DE GESTAO DE PESSOAS/PA</t>
-        </is>
-      </c>
-      <c r="D76">
-        <v>280649</v>
+          <t>DIVISAO DE GESTAO DE PESSOAS/SAMF/PA</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>212632</t>
+        </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>17000-000069321</t>
+          <t>17000-000063135</t>
         </is>
       </c>
     </row>
@@ -2272,15 +2422,17 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>DIVISAO DE GESTAO DE PESSOAS/SAMF/PA</t>
-        </is>
-      </c>
-      <c r="D77">
-        <v>212632</v>
+          <t>DIVISAO DE RECURSOS LOGISTICOS/PA</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>280650</t>
+        </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>17000-000063135</t>
+          <t>17000-000069322</t>
         </is>
       </c>
     </row>
@@ -2297,15 +2449,17 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>DIVISAO DE RECURSOS LOGISTICOS/PA</t>
-        </is>
-      </c>
-      <c r="D78">
-        <v>280650</v>
+          <t>SERV DE ATIVOS, INATIVOS E PENS/PA</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>280678</t>
+        </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>17000-000069322</t>
+          <t>17000-000069350</t>
         </is>
       </c>
     </row>
@@ -2322,15 +2476,17 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>SERV DE ATIVOS, INATIVOS E PENS/PA</t>
-        </is>
-      </c>
-      <c r="D79">
-        <v>280678</v>
+          <t>SERV. DE ORC. E FINANCAS/SAMF/PA</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>212629</t>
+        </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>17000-000069350</t>
+          <t>17000-000063132</t>
         </is>
       </c>
     </row>
@@ -2347,15 +2503,17 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>SERV. DE ORC. E FINANCAS/SAMF/PA</t>
-        </is>
-      </c>
-      <c r="D80">
-        <v>212629</v>
+          <t>SERVICO DE ATIVOS/DIGEP/SAMF/PA</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>212633</t>
+        </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>17000-000063132</t>
+          <t>17000-000063136</t>
         </is>
       </c>
     </row>
@@ -2372,15 +2530,17 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>SERVICO DE ATIVOS/DIGEP/SAMF/PA</t>
-        </is>
-      </c>
-      <c r="D81">
-        <v>212633</v>
+          <t>SERVICO DE INAT. E PENSION/DIGEP/SAMF/PA</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>212634</t>
+        </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>17000-000063136</t>
+          <t>17000-000063137</t>
         </is>
       </c>
     </row>
@@ -2397,15 +2557,17 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>SERVICO DE INAT. E PENSION/DIGEP/SAMF/PA</t>
-        </is>
-      </c>
-      <c r="D82">
-        <v>212634</v>
+          <t>SERVICO DE LICITACOES E CONTRATOS/PA</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>280677</t>
+        </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>17000-000063137</t>
+          <t>17000-000069349</t>
         </is>
       </c>
     </row>
@@ -2422,15 +2584,17 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>SERVICO DE LICITACOES E CONTRATOS/PA</t>
-        </is>
-      </c>
-      <c r="D83">
-        <v>280677</v>
+          <t>SERVICO DE SUPRIMENTOS/DRL/SAMF/PA</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>212631</t>
+        </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>17000-000069349</t>
+          <t>17000-000063134</t>
         </is>
       </c>
     </row>
@@ -2447,15 +2611,17 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>SERVICO DE SUPRIMENTOS/DRL/SAMF/PA</t>
-        </is>
-      </c>
-      <c r="D84">
-        <v>212631</v>
+          <t>SUPERINT REG DE ADMIN NO PARA</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>278708</t>
+        </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>17000-000063134</t>
+          <t>17000-000067380</t>
         </is>
       </c>
     </row>
@@ -2472,40 +2638,44 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>SUPERINT REG DE ADMIN NO PARA</t>
-        </is>
-      </c>
-      <c r="D85">
-        <v>278708</v>
+          <t>SUPERINTENDENCIA DE ADMINISTRACAO MF/PA</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>202708</t>
+        </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>17000-000067380</t>
+          <t>17000-000062000</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>PA</t>
+          <t>PB</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>SAMF/PA</t>
+          <t>SAMF/PB</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>SUPERINTENDENCIA DE ADMINISTRACAO MF/PA</t>
-        </is>
-      </c>
-      <c r="D86">
-        <v>202708</v>
+          <t>GEREN REG DE ADMIN NA PARAIBA</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>278720</t>
+        </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>17000-000062000</t>
+          <t>17000-000067392</t>
         </is>
       </c>
     </row>
@@ -2522,15 +2692,17 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>GEREN REG DE ADMIN NA PARAIBA</t>
-        </is>
-      </c>
-      <c r="D87">
-        <v>278720</v>
+          <t>SERVIC APOIO ADMINST DESCENTRALIZADA-PB</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>304914</t>
+        </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>17000-000067392</t>
+          <t>17000-000071906</t>
         </is>
       </c>
     </row>
@@ -2547,40 +2719,44 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>SERVIC APOIO ADMINST DESCENTRALIZADA-PB</t>
-        </is>
-      </c>
-      <c r="D88">
-        <v>304914</v>
+          <t>SUPERINTENDENCIA DE ADMINISTRACAO MF/PB</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>202698</t>
+        </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>17000-000071906</t>
+          <t>17000-000061990</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>PB</t>
+          <t>PE</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>SAMF/PB</t>
+          <t>SAMF/PE</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>SUPERINTENDENCIA DE ADMINISTRACAO MF/PB</t>
-        </is>
-      </c>
-      <c r="D89">
-        <v>202698</v>
+          <t>DIV. DE GESTAO DE PESSOAS/SAMF/PE</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>212646</t>
+        </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>17000-000061990</t>
+          <t>17000-000063149</t>
         </is>
       </c>
     </row>
@@ -2597,15 +2773,17 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>DIV. DE GESTAO DE PESSOAS/SAMF/PE</t>
-        </is>
-      </c>
-      <c r="D90">
-        <v>212646</v>
+          <t>DIV. DE PLAN. E CONTABILIDADE/SAMF/PE</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>212642</t>
+        </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>17000-000063149</t>
+          <t>17000-000063145</t>
         </is>
       </c>
     </row>
@@ -2622,15 +2800,17 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>DIV. DE PLAN. E CONTABILIDADE/SAMF/PE</t>
-        </is>
-      </c>
-      <c r="D91">
-        <v>212642</v>
+          <t>DIV. DE RECURSOS LOGISTICOS/SAMF/PE</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>212644</t>
+        </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>17000-000063145</t>
+          <t>17000-000063147</t>
         </is>
       </c>
     </row>
@@ -2647,15 +2827,17 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>DIV. DE RECURSOS LOGISTICOS/SAMF/PE</t>
-        </is>
-      </c>
-      <c r="D92">
-        <v>212644</v>
+          <t>DIVISAO DE GESTAO DE PESSOAS/PE</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>280652</t>
+        </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>17000-000063147</t>
+          <t>17000-000069324</t>
         </is>
       </c>
     </row>
@@ -2672,15 +2854,17 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>DIVISAO DE GESTAO DE PESSOAS/PE</t>
-        </is>
-      </c>
-      <c r="D93">
-        <v>280652</v>
+          <t>DIVISAO DE PLANEJAMENTO E ORCAMENTO/PE</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>280653</t>
+        </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>17000-000069324</t>
+          <t>17000-000069325</t>
         </is>
       </c>
     </row>
@@ -2697,15 +2881,17 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>DIVISAO DE PLANEJAMENTO E ORCAMENTO/PE</t>
-        </is>
-      </c>
-      <c r="D94">
-        <v>280653</v>
+          <t>DIVISAO DE RECURSOS LOGISTICOS/PE</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>280654</t>
+        </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>17000-000069325</t>
+          <t>17000-000069326</t>
         </is>
       </c>
     </row>
@@ -2722,15 +2908,17 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>DIVISAO DE RECURSOS LOGISTICOS/PE</t>
-        </is>
-      </c>
-      <c r="D95">
-        <v>280654</v>
+          <t>SERV. DE ORC. E FINANCAS/SAMF/PE</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>212643</t>
+        </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>17000-000069326</t>
+          <t>17000-000063146</t>
         </is>
       </c>
     </row>
@@ -2747,15 +2935,17 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>SERV. DE ORC. E FINANCAS/SAMF/PE</t>
-        </is>
-      </c>
-      <c r="D96">
-        <v>212643</v>
+          <t>SERVICO DE ATIVOS/DIGEP/SAMF/PE</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>212647</t>
+        </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>17000-000063146</t>
+          <t>17000-000063150</t>
         </is>
       </c>
     </row>
@@ -2772,15 +2962,17 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>SERVICO DE ATIVOS/DIGEP/SAMF/PE</t>
-        </is>
-      </c>
-      <c r="D97">
-        <v>212647</v>
+          <t>SERVICO DE INATIVOS E PENSIONISTAS/PE</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>280679</t>
+        </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>17000-000063150</t>
+          <t>17000-000069351</t>
         </is>
       </c>
     </row>
@@ -2797,15 +2989,17 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>SERVICO DE INATIVOS E PENSIONISTAS/PE</t>
-        </is>
-      </c>
-      <c r="D98">
-        <v>280679</v>
+          <t>SERVICO DE ORCAMENTO E FINANCAS/PE</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>280680</t>
+        </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>17000-000069351</t>
+          <t>17000-000069352</t>
         </is>
       </c>
     </row>
@@ -2822,15 +3016,17 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>SERVICO DE ORCAMENTO E FINANCAS/PE</t>
-        </is>
-      </c>
-      <c r="D99">
-        <v>280680</v>
+          <t>SERVICO DE SUPRIMENTOS/DRL/SAMF/PE</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>212645</t>
+        </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>17000-000069352</t>
+          <t>17000-000063148</t>
         </is>
       </c>
     </row>
@@ -2847,15 +3043,17 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>SERVICO DE SUPRIMENTOS/DRL/SAMF/PE</t>
-        </is>
-      </c>
-      <c r="D100">
-        <v>212645</v>
+          <t>SUPERINT REG DE ADMIN EM PERNAMBUCO</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>278702</t>
+        </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>17000-000063148</t>
+          <t>17000-000067374</t>
         </is>
       </c>
     </row>
@@ -2872,40 +3070,44 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>SUPERINT REG DE ADMIN EM PERNAMBUCO</t>
-        </is>
-      </c>
-      <c r="D101">
-        <v>278702</v>
+          <t>SUPERINTENDENCIA DE ADMINISTRACAO MF/PE</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>202694</t>
+        </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>17000-000067374</t>
+          <t>17000-000061986</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>PE</t>
+          <t>PI</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>SAMF/PE</t>
+          <t>SAMF/PI</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>SUPERINTENDENCIA DE ADMINISTRACAO MF/PE</t>
-        </is>
-      </c>
-      <c r="D102">
-        <v>202694</v>
+          <t>GEREN REG DE ADMIN DO ME NO EST DO PIAUI</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>278721</t>
+        </is>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>17000-000061986</t>
+          <t>17000-000067393</t>
         </is>
       </c>
     </row>
@@ -2922,15 +3124,17 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>GEREN REG DE ADMIN DO ME NO EST DO PIAUI</t>
-        </is>
-      </c>
-      <c r="D103">
-        <v>278721</v>
+          <t>SERVIC APOIO ADMINST DESCENTRALIZADA-PI</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>304905</t>
+        </is>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>17000-000067393</t>
+          <t>17000-000071897</t>
         </is>
       </c>
     </row>
@@ -2947,40 +3151,44 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>SERVIC APOIO ADMINST DESCENTRALIZADA-PI</t>
-        </is>
-      </c>
-      <c r="D104">
-        <v>304905</v>
+          <t>SUPERINTENDENCIA DE ADMINISTRACAO MF/PI</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>202699</t>
+        </is>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>17000-000071897</t>
+          <t>17000-000061991</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>PI</t>
+          <t>PR</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>SAMF/PI</t>
+          <t>SAMF/PR</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>SUPERINTENDENCIA DE ADMINISTRACAO MF/PI</t>
-        </is>
-      </c>
-      <c r="D105">
-        <v>202699</v>
+          <t>DIV DE PLANEJ, ORCAMENTO E FINANCAS</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>280655</t>
+        </is>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>17000-000061991</t>
+          <t>17000-000069327</t>
         </is>
       </c>
     </row>
@@ -2997,15 +3205,17 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>DIV DE PLANEJ, ORCAMENTO E FINANCAS</t>
-        </is>
-      </c>
-      <c r="D106">
-        <v>280655</v>
+          <t>DIV. DE REC. LOGISTICOS/SAMF/PR</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>212637</t>
+        </is>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>17000-000069327</t>
+          <t>17000-000063140</t>
         </is>
       </c>
     </row>
@@ -3022,15 +3232,17 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>DIV. DE REC. LOGISTICOS/SAMF/PR</t>
-        </is>
-      </c>
-      <c r="D107">
-        <v>212637</v>
+          <t>DIVISAO DA SUPERINTENDENCIA - SAMF/PR</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>203631</t>
+        </is>
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>17000-000063140</t>
+          <t>17000-000062055</t>
         </is>
       </c>
     </row>
@@ -3047,15 +3259,17 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>DIVISAO DA SUPERINTENDENCIA - SAMF/PR</t>
-        </is>
-      </c>
-      <c r="D108">
-        <v>203631</v>
+          <t>DIVISAO DE GESTAO DE PESSOAS</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>280656</t>
+        </is>
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>17000-000062055</t>
+          <t>17000-000069328</t>
         </is>
       </c>
     </row>
@@ -3072,15 +3286,17 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>DIVISAO DE GESTAO DE PESSOAS</t>
-        </is>
-      </c>
-      <c r="D109">
-        <v>280656</v>
+          <t>DIVISAO DE GESTAO DE PESSOAS/SAMF/PR</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>212639</t>
+        </is>
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>17000-000069328</t>
+          <t>17000-000063142</t>
         </is>
       </c>
     </row>
@@ -3097,15 +3313,17 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>DIVISAO DE GESTAO DE PESSOAS/SAMF/PR</t>
-        </is>
-      </c>
-      <c r="D110">
-        <v>212639</v>
+          <t>DIVISAO DE RECURSOS LOGISTICOS</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>280657</t>
+        </is>
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>17000-000063142</t>
+          <t>17000-000069329</t>
         </is>
       </c>
     </row>
@@ -3122,15 +3340,17 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>DIVISAO DE RECURSOS LOGISTICOS</t>
-        </is>
-      </c>
-      <c r="D111">
-        <v>280657</v>
+          <t>SERVICO DA SUPERINTENDENCIA - SAMF/PR</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>203636</t>
+        </is>
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>17000-000069329</t>
+          <t>17000-000062060</t>
         </is>
       </c>
     </row>
@@ -3147,15 +3367,17 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>SERVICO DA SUPERINTENDENCIA - SAMF/PR</t>
-        </is>
-      </c>
-      <c r="D112">
-        <v>203636</v>
+          <t>SERVICO DE APOIO 2</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>304836</t>
+        </is>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>17000-000062060</t>
+          <t>17000-000071817</t>
         </is>
       </c>
     </row>
@@ -3172,15 +3394,17 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>SERVICO DE APOIO 2</t>
-        </is>
-      </c>
-      <c r="D113">
-        <v>304836</v>
+          <t>SERVICO DE ORCAMENTO E FINANCAS</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>280682</t>
+        </is>
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>17000-000071817</t>
+          <t>17000-000069354</t>
         </is>
       </c>
     </row>
@@ -3197,15 +3421,17 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>SERVICO DE ORCAMENTO E FINANCAS</t>
-        </is>
-      </c>
-      <c r="D114">
-        <v>280682</v>
+          <t>SERVICO DE SUPRIMENTOS</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>280681</t>
+        </is>
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>17000-000069354</t>
+          <t>17000-000069353</t>
         </is>
       </c>
     </row>
@@ -3222,15 +3448,17 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>SERVICO DE SUPRIMENTOS</t>
-        </is>
-      </c>
-      <c r="D115">
-        <v>280681</v>
+          <t>SERVICO DE SUPRIMENTOS/DRL/SAMF/PR</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>212638</t>
+        </is>
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>17000-000069353</t>
+          <t>17000-000063141</t>
         </is>
       </c>
     </row>
@@ -3247,15 +3475,17 @@
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>SERVICO DE SUPRIMENTOS/DRL/SAMF/PR</t>
-        </is>
-      </c>
-      <c r="D116">
-        <v>212638</v>
+          <t>SUPERINT REG DE ADMIN NO PARANA</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>278703</t>
+        </is>
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>17000-000063141</t>
+          <t>17000-000067375</t>
         </is>
       </c>
     </row>
@@ -3272,40 +3502,44 @@
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>SUPERINT REG DE ADMIN NO PARANA</t>
-        </is>
-      </c>
-      <c r="D117">
-        <v>278703</v>
+          <t>SUPERINTENDENCIA DE ADMINISTRACAO MF/PR</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>202703</t>
+        </is>
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>17000-000067375</t>
+          <t>17000-000061995</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>PR</t>
+          <t>RJ</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>SAMF/PR</t>
+          <t>SAMF/RJ</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>SUPERINTENDENCIA DE ADMINISTRACAO MF/PR</t>
-        </is>
-      </c>
-      <c r="D118">
-        <v>202703</v>
+          <t>DIV DE APOIO EM ADMIN E LOGISTICA-RJ</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>304915</t>
+        </is>
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>17000-000061995</t>
+          <t>17000-000071907</t>
         </is>
       </c>
     </row>
@@ -3322,15 +3556,17 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>DIV DE APOIO EM ADMIN E LOGISTICA-RJ</t>
-        </is>
-      </c>
-      <c r="D119">
-        <v>304915</v>
+          <t>DIV DE APOIO EM GESTAO DE PESSOAS-RJ</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>304913</t>
+        </is>
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>17000-000071907</t>
+          <t>17000-000071905</t>
         </is>
       </c>
     </row>
@@ -3347,15 +3583,17 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>DIV DE APOIO EM GESTAO DE PESSOAS-RJ</t>
-        </is>
-      </c>
-      <c r="D120">
-        <v>304913</v>
+          <t>GERENCIA DE GESTAO DE PESSOAS</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>280629</t>
+        </is>
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>17000-000071905</t>
+          <t>17000-000069301</t>
         </is>
       </c>
     </row>
@@ -3372,15 +3610,17 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>GERENCIA DE GESTAO DE PESSOAS</t>
-        </is>
-      </c>
-      <c r="D121">
-        <v>280629</v>
+          <t>GERENCIA DE ORCAMENTO E FINANCAS</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>280630</t>
+        </is>
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>17000-000069301</t>
+          <t>17000-000069302</t>
         </is>
       </c>
     </row>
@@ -3397,15 +3637,17 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>GERENCIA DE ORCAMENTO E FINANCAS</t>
-        </is>
-      </c>
-      <c r="D122">
-        <v>280630</v>
+          <t>GERENCIA DE RECURSOS LOGISTICOS</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>280628</t>
+        </is>
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>17000-000069302</t>
+          <t>17000-000069300</t>
         </is>
       </c>
     </row>
@@ -3422,15 +3664,17 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>GERENCIA DE RECURSOS LOGISTICOS</t>
-        </is>
-      </c>
-      <c r="D123">
-        <v>280628</v>
+          <t>SERVICO DE ATIVOS</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>280685</t>
+        </is>
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>17000-000069300</t>
+          <t>17000-000069357</t>
         </is>
       </c>
     </row>
@@ -3447,15 +3691,17 @@
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>SERVICO DE ATIVOS</t>
-        </is>
-      </c>
-      <c r="D124">
-        <v>280685</v>
+          <t>SERVICO DE INATIVOS E PENSIONISTAS</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>280684</t>
+        </is>
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>17000-000069357</t>
+          <t>17000-000069356</t>
         </is>
       </c>
     </row>
@@ -3472,15 +3718,17 @@
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>SERVICO DE INATIVOS E PENSIONISTAS</t>
-        </is>
-      </c>
-      <c r="D125">
-        <v>280684</v>
+          <t>SERVICO DE ORCAMENTO E FINANCAS</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>280686</t>
+        </is>
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>17000-000069356</t>
+          <t>17000-000069358</t>
         </is>
       </c>
     </row>
@@ -3497,15 +3745,17 @@
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>SERVICO DE ORCAMENTO E FINANCAS</t>
-        </is>
-      </c>
-      <c r="D126">
-        <v>280686</v>
+          <t>SERVICO DE SUPRIMENTOS</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>280683</t>
+        </is>
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>17000-000069358</t>
+          <t>17000-000069355</t>
         </is>
       </c>
     </row>
@@ -3522,15 +3772,17 @@
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>SERVICO DE SUPRIMENTOS</t>
-        </is>
-      </c>
-      <c r="D127">
-        <v>280683</v>
+          <t>SUPERINT REG DE ADMIN NO RIO DE JANEIRO</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>278700</t>
+        </is>
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>17000-000069355</t>
+          <t>17000-000067372</t>
         </is>
       </c>
     </row>
@@ -3547,40 +3799,44 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>SUPERINT REG DE ADMIN NO RIO DE JANEIRO</t>
-        </is>
-      </c>
-      <c r="D128">
-        <v>278700</v>
+          <t>SUPERINTENDENCIA DE ADMINISTRACAO MF/RJ</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>202692</t>
+        </is>
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>17000-000067372</t>
+          <t>17000-000061984</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>RJ</t>
+          <t>RN</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>SAMF/RJ</t>
+          <t>SAMF/RN</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>SUPERINTENDENCIA DE ADMINISTRACAO MF/RJ</t>
-        </is>
-      </c>
-      <c r="D129">
-        <v>202692</v>
+          <t>GEREN REG DE ADM NO RIO GRANDE DO NORTE</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>278722</t>
+        </is>
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>17000-000061984</t>
+          <t>17000-000067394</t>
         </is>
       </c>
     </row>
@@ -3597,15 +3853,17 @@
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>GEREN REG DE ADM NO RIO GRANDE DO NORTE</t>
-        </is>
-      </c>
-      <c r="D130">
-        <v>278722</v>
+          <t>SERVIC APOIO ADMINST DESCENTRALIZADA-RN</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>304860</t>
+        </is>
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>17000-000067394</t>
+          <t>17000-000071841</t>
         </is>
       </c>
     </row>
@@ -3622,90 +3880,98 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>SERVIC APOIO ADMINST DESCENTRALIZADA-RN</t>
-        </is>
-      </c>
-      <c r="D131">
-        <v>304860</v>
+          <t>SUPERINTENDENCIA DE ADMINISTRACAO MF/RN</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>202700</t>
+        </is>
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>17000-000071841</t>
+          <t>17000-000061992</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>RN</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>SAMF/RN</t>
+          <t>SAMF/RO</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>SUPERINTENDENCIA DE ADMINISTRACAO MF/RN</t>
-        </is>
-      </c>
-      <c r="D132">
-        <v>202700</v>
+          <t>SUPERINTENDENCIA DE ADMINISTRACAO MF/RO</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>202713</t>
+        </is>
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>17000-000061992</t>
+          <t>17000-000062005</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>RO</t>
+          <t>RR</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>SAMF/RO</t>
+          <t>SAMF/RR</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>SUPERINTENDENCIA DE ADMINISTRACAO MF/RO</t>
-        </is>
-      </c>
-      <c r="D133">
-        <v>202713</v>
+          <t>SUPERINTENDENCIA DE ADMINISTRACAO MF/RR</t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>202714</t>
+        </is>
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>17000-000062005</t>
+          <t>17000-000062006</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>RR</t>
+          <t>RS</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>SAMF/RR</t>
+          <t>SAMF/RS</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>SUPERINTENDENCIA DE ADMINISTRACAO MF/RR</t>
-        </is>
-      </c>
-      <c r="D134">
-        <v>202714</v>
+          <t>DIVISAO DE GESTAO DE PESSOAS</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>280660</t>
+        </is>
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>17000-000062006</t>
+          <t>17000-000069332</t>
         </is>
       </c>
     </row>
@@ -3722,15 +3988,17 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>DIVISAO DE GESTAO DE PESSOAS</t>
-        </is>
-      </c>
-      <c r="D135">
-        <v>280660</v>
+          <t>DIVISAO DE PLANEJAMENTO E ORCAMENTO</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>280658</t>
+        </is>
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>17000-000069332</t>
+          <t>17000-000069330</t>
         </is>
       </c>
     </row>
@@ -3747,15 +4015,17 @@
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>DIVISAO DE PLANEJAMENTO E ORCAMENTO</t>
-        </is>
-      </c>
-      <c r="D136">
-        <v>280658</v>
+          <t>DIVISAO DE RECURSOS LOGISTICOS</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>280659</t>
+        </is>
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>17000-000069330</t>
+          <t>17000-000069331</t>
         </is>
       </c>
     </row>
@@ -3772,15 +4042,17 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>DIVISAO DE RECURSOS LOGISTICOS</t>
-        </is>
-      </c>
-      <c r="D137">
-        <v>280659</v>
+          <t>SERVICO DE ORCAMENTO E FINANCAS</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>280688</t>
+        </is>
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>17000-000069331</t>
+          <t>17000-000069360</t>
         </is>
       </c>
     </row>
@@ -3797,15 +4069,17 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>SERVICO DE ORCAMENTO E FINANCAS</t>
-        </is>
-      </c>
-      <c r="D138">
-        <v>280688</v>
+          <t>SERVICO DE SUPRIMENTOS</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>280687</t>
+        </is>
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>17000-000069360</t>
+          <t>17000-000069359</t>
         </is>
       </c>
     </row>
@@ -3822,15 +4096,17 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>SERVICO DE SUPRIMENTOS</t>
-        </is>
-      </c>
-      <c r="D139">
-        <v>280687</v>
+          <t>SUPERINT REG DE ADM NO RIO GRANDE DO SUL</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>278704</t>
+        </is>
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>17000-000069359</t>
+          <t>17000-000067376</t>
         </is>
       </c>
     </row>
@@ -3847,40 +4123,44 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>SUPERINT REG DE ADM NO RIO GRANDE DO SUL</t>
-        </is>
-      </c>
-      <c r="D140">
-        <v>278704</v>
+          <t>SUPERINTENDENCIA DE ADMINISTRACAO MF/RS</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>202704</t>
+        </is>
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>17000-000067376</t>
+          <t>17000-000061996</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>RS</t>
+          <t>SC</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>SAMF/RS</t>
+          <t>SAMF/SC</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>SUPERINTENDENCIA DE ADMINISTRACAO MF/RS</t>
-        </is>
-      </c>
-      <c r="D141">
-        <v>202704</v>
+          <t>GEREN REG DE ADMIN EM SANTA CATARINA</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>278723</t>
+        </is>
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>17000-000061996</t>
+          <t>17000-000067395</t>
         </is>
       </c>
     </row>
@@ -3897,15 +4177,17 @@
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>GEREN REG DE ADMIN EM SANTA CATARINA</t>
-        </is>
-      </c>
-      <c r="D142">
-        <v>278723</v>
+          <t>SERVIC APOIO ADMINST DESCENTRALIZADA-SC</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>304861</t>
+        </is>
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>17000-000067395</t>
+          <t>17000-000071842</t>
         </is>
       </c>
     </row>
@@ -3922,40 +4204,44 @@
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>SERVIC APOIO ADMINST DESCENTRALIZADA-SC</t>
-        </is>
-      </c>
-      <c r="D143">
-        <v>304861</v>
+          <t>SUPERINTENDENCIA DE ADMINISTRACAO MF/SC</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>202701</t>
+        </is>
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>17000-000071842</t>
+          <t>17000-000061993</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>SC</t>
+          <t>SE</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>SAMF/SC</t>
+          <t>SAMF/SE</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>SUPERINTENDENCIA DE ADMINISTRACAO MF/SC</t>
-        </is>
-      </c>
-      <c r="D144">
-        <v>202701</v>
+          <t>GEREN REG DE ADMIN EM SERGIPE</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>278724</t>
+        </is>
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>17000-000061993</t>
+          <t>17000-000067396</t>
         </is>
       </c>
     </row>
@@ -3972,15 +4258,17 @@
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>GEREN REG DE ADMIN EM SERGIPE</t>
-        </is>
-      </c>
-      <c r="D145">
-        <v>278724</v>
+          <t>SERVIC APOIO ADMINST DESCENTRALIZADA-SE</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>304917</t>
+        </is>
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>17000-000067396</t>
+          <t>17000-000071909</t>
         </is>
       </c>
     </row>
@@ -3997,40 +4285,44 @@
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>SERVIC APOIO ADMINST DESCENTRALIZADA-SE</t>
-        </is>
-      </c>
-      <c r="D146">
-        <v>304917</v>
+          <t>SUPERINTENDENCIA DE ADMINISTRACAO MF/SE</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>202702</t>
+        </is>
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t>17000-000071909</t>
+          <t>17000-000061994</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>SE</t>
+          <t>SP</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>SAMF/SE</t>
+          <t>SAMF/SP</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>SUPERINTENDENCIA DE ADMINISTRACAO MF/SE</t>
-        </is>
-      </c>
-      <c r="D147">
-        <v>202702</v>
+          <t>COORD DO ESCRIT DE UNID DESC-SAO PAULO</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>285288</t>
+        </is>
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t>17000-000061994</t>
+          <t>17000-000069723</t>
         </is>
       </c>
     </row>
@@ -4047,15 +4339,17 @@
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>COORD DO ESCRIT DE UNID DESC-SAO PAULO</t>
-        </is>
-      </c>
-      <c r="D148">
-        <v>285288</v>
+          <t>DIV. DE PLANEJ. E CONTABILIDADE/SAMF/SP</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>212656</t>
+        </is>
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t>17000-000069723</t>
+          <t>17000-000063159</t>
         </is>
       </c>
     </row>
@@ -4072,15 +4366,17 @@
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>DIV. DE PLANEJ. E CONTABILIDADE/SAMF/SP</t>
-        </is>
-      </c>
-      <c r="D149">
-        <v>212656</v>
+          <t>DIVISAO DE GESTAO DE PESSOAS</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>280663</t>
+        </is>
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>17000-000063159</t>
+          <t>17000-000069335</t>
         </is>
       </c>
     </row>
@@ -4097,15 +4393,17 @@
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>DIVISAO DE GESTAO DE PESSOAS</t>
-        </is>
-      </c>
-      <c r="D150">
-        <v>280663</v>
+          <t>DIVISAO DE GESTAO DE PESSOAS/SAMF/SP</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>212660</t>
+        </is>
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>17000-000069335</t>
+          <t>17000-000063163</t>
         </is>
       </c>
     </row>
@@ -4122,15 +4420,17 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>DIVISAO DE GESTAO DE PESSOAS/SAMF/SP</t>
-        </is>
-      </c>
-      <c r="D151">
-        <v>212660</v>
+          <t>DIVISAO DE PLANEJAMENTO E ORCAMENTO</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>280661</t>
+        </is>
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t>17000-000063163</t>
+          <t>17000-000069333</t>
         </is>
       </c>
     </row>
@@ -4147,15 +4447,17 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>DIVISAO DE PLANEJAMENTO E ORCAMENTO</t>
-        </is>
-      </c>
-      <c r="D152">
-        <v>280661</v>
+          <t>DIVISAO DE RECURSOS LOGISTICOS</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>280662</t>
+        </is>
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>17000-000069333</t>
+          <t>17000-000069334</t>
         </is>
       </c>
     </row>
@@ -4172,15 +4474,17 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>DIVISAO DE RECURSOS LOGISTICOS</t>
-        </is>
-      </c>
-      <c r="D153">
-        <v>280662</v>
+          <t>DIVISAO DE RECURSOS LOGISTICOS/SAMF/SP</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>212658</t>
+        </is>
       </c>
       <c r="E153" t="inlineStr">
         <is>
-          <t>17000-000069334</t>
+          <t>17000-000063161</t>
         </is>
       </c>
     </row>
@@ -4197,15 +4501,17 @@
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>DIVISAO DE RECURSOS LOGISTICOS/SAMF/SP</t>
-        </is>
-      </c>
-      <c r="D154">
-        <v>212658</v>
+          <t>SERV. DE INAT. E PENSION./DIGEP/SAMF/SP</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>212662</t>
+        </is>
       </c>
       <c r="E154" t="inlineStr">
         <is>
-          <t>17000-000063161</t>
+          <t>17000-000063165</t>
         </is>
       </c>
     </row>
@@ -4222,15 +4528,17 @@
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>SERV. DE INAT. E PENSION./DIGEP/SAMF/SP</t>
-        </is>
-      </c>
-      <c r="D155">
-        <v>212662</v>
+          <t>SERV. DE ORC. E FINANCAS/SAMF/SP</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>212657</t>
+        </is>
       </c>
       <c r="E155" t="inlineStr">
         <is>
-          <t>17000-000063165</t>
+          <t>17000-000063160</t>
         </is>
       </c>
     </row>
@@ -4247,15 +4555,17 @@
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>SERV. DE ORC. E FINANCAS/SAMF/SP</t>
-        </is>
-      </c>
-      <c r="D156">
-        <v>212657</v>
+          <t>SERVICO DE ATIVOS</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>280690</t>
+        </is>
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t>17000-000063160</t>
+          <t>17000-000069362</t>
         </is>
       </c>
     </row>
@@ -4272,15 +4582,17 @@
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>SERVICO DE ATIVOS</t>
-        </is>
-      </c>
-      <c r="D157">
-        <v>280690</v>
+          <t>SERVICO DE ATIVOS/DIGEP/SAMF/SP</t>
+        </is>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>212661</t>
+        </is>
       </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t>17000-000069362</t>
+          <t>17000-000063164</t>
         </is>
       </c>
     </row>
@@ -4297,15 +4609,17 @@
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>SERVICO DE ATIVOS/DIGEP/SAMF/SP</t>
-        </is>
-      </c>
-      <c r="D158">
-        <v>212661</v>
+          <t>SERVICO DE INATIVOS E PENSIONISTAS</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>280691</t>
+        </is>
       </c>
       <c r="E158" t="inlineStr">
         <is>
-          <t>17000-000063164</t>
+          <t>17000-000069363</t>
         </is>
       </c>
     </row>
@@ -4322,15 +4636,17 @@
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>SERVICO DE INATIVOS E PENSIONISTAS</t>
-        </is>
-      </c>
-      <c r="D159">
-        <v>280691</v>
+          <t>SERVICO DE ORCAMENTO E FINANCAS</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>280689</t>
+        </is>
       </c>
       <c r="E159" t="inlineStr">
         <is>
-          <t>17000-000069363</t>
+          <t>17000-000069361</t>
         </is>
       </c>
     </row>
@@ -4347,15 +4663,17 @@
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>SERVICO DE ORCAMENTO E FINANCAS</t>
-        </is>
-      </c>
-      <c r="D160">
-        <v>280689</v>
+          <t>SERVICO DE SUPRIMENTOS</t>
+        </is>
+      </c>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>280692</t>
+        </is>
       </c>
       <c r="E160" t="inlineStr">
         <is>
-          <t>17000-000069361</t>
+          <t>17000-000069364</t>
         </is>
       </c>
     </row>
@@ -4372,15 +4690,17 @@
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>SERVICO DE SUPRIMENTOS</t>
-        </is>
-      </c>
-      <c r="D161">
-        <v>280692</v>
+          <t>SERVICO DE SUPRIMENTOS/DRL/SAMF/SP</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>212659</t>
+        </is>
       </c>
       <c r="E161" t="inlineStr">
         <is>
-          <t>17000-000069364</t>
+          <t>17000-000063162</t>
         </is>
       </c>
     </row>
@@ -4397,15 +4717,17 @@
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>SERVICO DE SUPRIMENTOS/DRL/SAMF/SP</t>
-        </is>
-      </c>
-      <c r="D162">
-        <v>212659</v>
+          <t>SUPERINT REG DE ADMIN EM SAO PAULO</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>278705</t>
+        </is>
       </c>
       <c r="E162" t="inlineStr">
         <is>
-          <t>17000-000063162</t>
+          <t>17000-000067377</t>
         </is>
       </c>
     </row>
@@ -4422,40 +4744,44 @@
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>SUPERINT REG DE ADMIN EM SAO PAULO</t>
-        </is>
-      </c>
-      <c r="D163">
-        <v>278705</v>
+          <t>SUPERINTENDENCIA DE ADMINISTRACAO MF/SP</t>
+        </is>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>202705</t>
+        </is>
       </c>
       <c r="E163" t="inlineStr">
         <is>
-          <t>17000-000067377</t>
+          <t>17000-000061997</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>SP</t>
+          <t>AL</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>SAMF/SP</t>
+          <t>SAMF/AL</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>SUPERINTENDENCIA DE ADMINISTRACAO MF/SP</t>
-        </is>
-      </c>
-      <c r="D164">
-        <v>202705</v>
+          <t>GEREN REG DE ADMIN EM ALAGOAS</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>278715</t>
+        </is>
       </c>
       <c r="E164" t="inlineStr">
         <is>
-          <t>17000-000061997</t>
+          <t>17000-000067387</t>
         </is>
       </c>
     </row>

</xml_diff>